<commit_message>
Added lat lon decimal conversions
</commit_message>
<xml_diff>
--- a/DATA/locality_data.xlsx
+++ b/DATA/locality_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\britt\Desktop\GIT _SUBMIT\Project-2\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\Git\Project-2\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5EE9AA2-03FD-4E37-8EB4-DFA270D891E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F715AABA-36F3-4D50-997F-4F4B1CA2D710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-4908" windowWidth="23232" windowHeight="12696" xr2:uid="{62C98334-B8DE-4504-A4BC-6B0F5A016A6A}"/>
+    <workbookView xWindow="-10020" yWindow="1500" windowWidth="21600" windowHeight="11385" xr2:uid="{62C98334-B8DE-4504-A4BC-6B0F5A016A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
   <si>
     <t>Suborder Publish Year</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Ain Dara, Caza Aley, Lebanese amber</t>
+  </si>
+  <si>
+    <t>Lat_dec</t>
+  </si>
+  <si>
+    <t>Lon_dec</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A609E2-1CEE-46A8-9788-8933E11F2F49}">
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,39 +693,41 @@
     <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="63.5703125" style="1" customWidth="1"/>
-    <col min="15" max="24" width="93.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="52" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="63.5703125" style="1" customWidth="1"/>
+    <col min="17" max="26" width="93.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="54" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -750,50 +758,56 @@
       <c r="J1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -824,50 +838,56 @@
       <c r="J2" s="1">
         <v>1917</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>96.583330000000004</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AA2" s="1">
         <v>1992</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>1894</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AG2" s="1">
         <v>1894</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AJ2" s="1">
         <v>1917</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -898,50 +918,56 @@
       <c r="J3" s="1">
         <v>2009</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="1">
+        <v>45.933</v>
+      </c>
+      <c r="L3" s="1">
+        <v>-0.66400000000000003</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="AA3" s="1">
         <v>1992</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AD3" s="1">
         <v>1826</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AG3" s="1">
         <v>1827</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AJ3" s="1">
         <v>2009</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -972,50 +998,56 @@
       <c r="J4" s="1">
         <v>1920</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>96.583330000000004</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <v>1992</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AD4" s="1">
         <v>1879</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AG4" s="1">
         <v>1888</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AJ4" s="1">
         <v>1898</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1046,20 +1078,26 @@
       <c r="J5" s="1">
         <v>2016</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>96.583330000000004</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1090,20 +1128,26 @@
       <c r="J6" s="1">
         <v>2009</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="1">
+        <v>45.933</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-0.66400000000000003</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1134,20 +1178,26 @@
       <c r="J7" s="1">
         <v>2002</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="1">
+        <v>40.450000000000003</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-74.349999999999994</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1178,20 +1228,26 @@
       <c r="J8" s="1">
         <v>1991</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="1">
+        <v>49.816600000000001</v>
+      </c>
+      <c r="L8" s="1">
+        <v>-111.6833</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,20 +1278,26 @@
       <c r="J9" s="1">
         <v>1980</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="1">
+        <v>33.133299999999998</v>
+      </c>
+      <c r="L9" s="1">
+        <v>-35.583329999999997</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1266,20 +1328,26 @@
       <c r="J10" s="1">
         <v>2007</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="1">
+        <v>46.2333</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-2.6833300000000002</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,16 +1378,22 @@
       <c r="J11" s="1">
         <v>2020</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="L11" s="1">
+        <v>96.583330000000004</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>